<commit_message>
label, sound, music, voice, transition, pause, scene
</commit_message>
<xml_diff>
--- a/test/RenpyData.xlsx
+++ b/test/RenpyData.xlsx
@@ -6,7 +6,7 @@
     <sheet state="visible" name="Character" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Image" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="CustomCode" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="start" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Chapter0" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="294">
   <si>
     <t>Variable</t>
   </si>
@@ -803,46 +803,55 @@
         linear 3.0 rotate 360
         repeat
 init:
-    $ my_center = Position(xpos= 0.5, xanchor='center' )
-    $ h_center = Position(xpos= 0.46, xanchor='center' )
-    $ my_left = Position(xpos= 0.1, xanchor='left')
-    $ my_right = Position(xpos= 0.9, xanchor='right')
+    $ custom_center = Position(xpos= 0.5, xanchor='center' )
+    $ hetris_center = Position(xpos= 0.46, xanchor='center' )
+    $ custom_left = Position(xpos= 0.1, xanchor='left')
+    $ custom_right = Position(xpos= 0.9, xanchor='right')
 </t>
   </si>
   <si>
     <t>Label</t>
   </si>
   <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Sound</t>
+  </si>
+  <si>
+    <t>Scene</t>
+  </si>
+  <si>
+    <t>Voice</t>
+  </si>
+  <si>
+    <t>Tachie</t>
+  </si>
+  <si>
+    <t>TachiePosition</t>
+  </si>
+  <si>
+    <t>IsOption</t>
+  </si>
+  <si>
     <t>Character</t>
   </si>
   <si>
     <t>Dialog</t>
   </si>
   <si>
-    <t>Music</t>
-  </si>
-  <si>
-    <t>Tachie</t>
-  </si>
-  <si>
-    <t>TachiePosition</t>
-  </si>
-  <si>
-    <t>Background</t>
+    <t>HideTachieAfterward</t>
+  </si>
+  <si>
+    <t>HideTachieAtPos</t>
   </si>
   <si>
     <t>Transition</t>
   </si>
   <si>
-    <t>Sound</t>
-  </si>
-  <si>
     <t>SpecialEffect</t>
   </si>
   <si>
-    <t>Voice</t>
-  </si>
-  <si>
     <t>JumpToLabel</t>
   </si>
   <si>
@@ -852,6 +861,9 @@
     <t>Pause</t>
   </si>
   <si>
+    <t>RenpyCommand</t>
+  </si>
+  <si>
     <t>Remark</t>
   </si>
   <si>
@@ -870,25 +882,25 @@
     <t>dissolve</t>
   </si>
   <si>
+    <t>metro_arriving</t>
+  </si>
+  <si>
     <t>mtr1</t>
   </si>
   <si>
     <t>fade</t>
   </si>
   <si>
-    <t>metro_arriving</t>
-  </si>
-  <si>
     <t>narrator_adv</t>
   </si>
   <si>
     <t>請勿靠近車門</t>
   </si>
   <si>
+    <t>footstep</t>
+  </si>
+  <si>
     <t>我拖著行李下車，小心翼翼地穿梭在人群中。</t>
-  </si>
-  <si>
-    <t>footstep</t>
   </si>
   <si>
     <t>street</t>
@@ -929,7 +941,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -940,6 +952,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF93C47D"/>
+        <bgColor rgb="FF93C47D"/>
       </patternFill>
     </fill>
     <fill>
@@ -955,7 +973,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -974,6 +992,10 @@
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -2371,10 +2393,10 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="154.75"/>
+    <col customWidth="1" min="1" max="1" width="207.88"/>
   </cols>
   <sheetData>
-    <row r="1" ht="331.5" customHeight="1">
+    <row r="1" ht="420.0" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>259</v>
       </c>
@@ -2397,10 +2419,16 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="41.0"/>
-    <col customWidth="1" min="9" max="9" width="16.38"/>
-    <col customWidth="1" min="13" max="13" width="8.5"/>
-    <col customWidth="1" min="14" max="14" width="5.75"/>
+    <col customWidth="1" min="3" max="3" width="16.38"/>
+    <col customWidth="1" min="5" max="5" width="14.5"/>
+    <col customWidth="1" min="7" max="7" width="16.13"/>
+    <col customWidth="1" min="10" max="10" width="41.0"/>
+    <col customWidth="1" min="11" max="11" width="16.88"/>
+    <col customWidth="1" min="12" max="12" width="18.38"/>
+    <col customWidth="1" min="17" max="17" width="8.0"/>
+    <col customWidth="1" min="18" max="18" width="15.38"/>
+    <col customWidth="1" min="19" max="19" width="21.88"/>
+    <col customWidth="1" min="20" max="20" width="20.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2416,16 +2444,16 @@
       <c r="D1" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>267</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -2446,77 +2474,3085 @@
       <c r="N1" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="1" t="s">
         <v>274</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>275</v>
+        <v>279</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>281</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>277</v>
+        <v>282</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="G3" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="N3" s="1">
-        <v>3.0</v>
+      <c r="C3" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="M3" s="1" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="4">
-      <c r="G4" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>281</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>282</v>
+        <v>287</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>283</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>284</v>
+        <v>289</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="J5" s="1" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="6">
-      <c r="C6" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="M6" s="1" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="7">
-      <c r="G7" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>281</v>
-      </c>
+      <c r="B7" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="G7" s="7"/>
     </row>
     <row r="8">
-      <c r="D8" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>289</v>
-      </c>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9">
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10">
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11">
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12">
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13">
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14">
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15">
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16">
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17">
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18">
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19">
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20">
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21">
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22">
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23">
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24">
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25">
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26">
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27">
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28">
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29">
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30">
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31">
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32">
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33">
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34">
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35">
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36">
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37">
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38">
+      <c r="G38" s="7"/>
+    </row>
+    <row r="39">
+      <c r="G39" s="7"/>
+    </row>
+    <row r="40">
+      <c r="G40" s="7"/>
+    </row>
+    <row r="41">
+      <c r="G41" s="7"/>
+    </row>
+    <row r="42">
+      <c r="G42" s="7"/>
+    </row>
+    <row r="43">
+      <c r="G43" s="7"/>
+    </row>
+    <row r="44">
+      <c r="G44" s="7"/>
+    </row>
+    <row r="45">
+      <c r="G45" s="7"/>
+    </row>
+    <row r="46">
+      <c r="G46" s="7"/>
+    </row>
+    <row r="47">
+      <c r="G47" s="7"/>
+    </row>
+    <row r="48">
+      <c r="G48" s="7"/>
+    </row>
+    <row r="49">
+      <c r="G49" s="7"/>
+    </row>
+    <row r="50">
+      <c r="G50" s="7"/>
+    </row>
+    <row r="51">
+      <c r="G51" s="7"/>
+    </row>
+    <row r="52">
+      <c r="G52" s="7"/>
+    </row>
+    <row r="53">
+      <c r="G53" s="7"/>
+    </row>
+    <row r="54">
+      <c r="G54" s="7"/>
+    </row>
+    <row r="55">
+      <c r="G55" s="7"/>
+    </row>
+    <row r="56">
+      <c r="G56" s="7"/>
+    </row>
+    <row r="57">
+      <c r="G57" s="7"/>
+    </row>
+    <row r="58">
+      <c r="G58" s="7"/>
+    </row>
+    <row r="59">
+      <c r="G59" s="7"/>
+    </row>
+    <row r="60">
+      <c r="G60" s="7"/>
+    </row>
+    <row r="61">
+      <c r="G61" s="7"/>
+    </row>
+    <row r="62">
+      <c r="G62" s="7"/>
+    </row>
+    <row r="63">
+      <c r="G63" s="7"/>
+    </row>
+    <row r="64">
+      <c r="G64" s="7"/>
+    </row>
+    <row r="65">
+      <c r="G65" s="7"/>
+    </row>
+    <row r="66">
+      <c r="G66" s="7"/>
+    </row>
+    <row r="67">
+      <c r="G67" s="7"/>
+    </row>
+    <row r="68">
+      <c r="G68" s="7"/>
+    </row>
+    <row r="69">
+      <c r="G69" s="7"/>
+    </row>
+    <row r="70">
+      <c r="G70" s="7"/>
+    </row>
+    <row r="71">
+      <c r="G71" s="7"/>
+    </row>
+    <row r="72">
+      <c r="G72" s="7"/>
+    </row>
+    <row r="73">
+      <c r="G73" s="7"/>
+    </row>
+    <row r="74">
+      <c r="G74" s="7"/>
+    </row>
+    <row r="75">
+      <c r="G75" s="7"/>
+    </row>
+    <row r="76">
+      <c r="G76" s="7"/>
+    </row>
+    <row r="77">
+      <c r="G77" s="7"/>
+    </row>
+    <row r="78">
+      <c r="G78" s="7"/>
+    </row>
+    <row r="79">
+      <c r="G79" s="7"/>
+    </row>
+    <row r="80">
+      <c r="G80" s="7"/>
+    </row>
+    <row r="81">
+      <c r="G81" s="7"/>
+    </row>
+    <row r="82">
+      <c r="G82" s="7"/>
+    </row>
+    <row r="83">
+      <c r="G83" s="7"/>
+    </row>
+    <row r="84">
+      <c r="G84" s="7"/>
+    </row>
+    <row r="85">
+      <c r="G85" s="7"/>
+    </row>
+    <row r="86">
+      <c r="G86" s="7"/>
+    </row>
+    <row r="87">
+      <c r="G87" s="7"/>
+    </row>
+    <row r="88">
+      <c r="G88" s="7"/>
+    </row>
+    <row r="89">
+      <c r="G89" s="7"/>
+    </row>
+    <row r="90">
+      <c r="G90" s="7"/>
+    </row>
+    <row r="91">
+      <c r="G91" s="7"/>
+    </row>
+    <row r="92">
+      <c r="G92" s="7"/>
+    </row>
+    <row r="93">
+      <c r="G93" s="7"/>
+    </row>
+    <row r="94">
+      <c r="G94" s="7"/>
+    </row>
+    <row r="95">
+      <c r="G95" s="7"/>
+    </row>
+    <row r="96">
+      <c r="G96" s="7"/>
+    </row>
+    <row r="97">
+      <c r="G97" s="7"/>
+    </row>
+    <row r="98">
+      <c r="G98" s="7"/>
+    </row>
+    <row r="99">
+      <c r="G99" s="7"/>
+    </row>
+    <row r="100">
+      <c r="G100" s="7"/>
+    </row>
+    <row r="101">
+      <c r="G101" s="7"/>
+    </row>
+    <row r="102">
+      <c r="G102" s="7"/>
+    </row>
+    <row r="103">
+      <c r="G103" s="7"/>
+    </row>
+    <row r="104">
+      <c r="G104" s="7"/>
+    </row>
+    <row r="105">
+      <c r="G105" s="7"/>
+    </row>
+    <row r="106">
+      <c r="G106" s="7"/>
+    </row>
+    <row r="107">
+      <c r="G107" s="7"/>
+    </row>
+    <row r="108">
+      <c r="G108" s="7"/>
+    </row>
+    <row r="109">
+      <c r="G109" s="7"/>
+    </row>
+    <row r="110">
+      <c r="G110" s="7"/>
+    </row>
+    <row r="111">
+      <c r="G111" s="7"/>
+    </row>
+    <row r="112">
+      <c r="G112" s="7"/>
+    </row>
+    <row r="113">
+      <c r="G113" s="7"/>
+    </row>
+    <row r="114">
+      <c r="G114" s="7"/>
+    </row>
+    <row r="115">
+      <c r="G115" s="7"/>
+    </row>
+    <row r="116">
+      <c r="G116" s="7"/>
+    </row>
+    <row r="117">
+      <c r="G117" s="7"/>
+    </row>
+    <row r="118">
+      <c r="G118" s="7"/>
+    </row>
+    <row r="119">
+      <c r="G119" s="7"/>
+    </row>
+    <row r="120">
+      <c r="G120" s="7"/>
+    </row>
+    <row r="121">
+      <c r="G121" s="7"/>
+    </row>
+    <row r="122">
+      <c r="G122" s="7"/>
+    </row>
+    <row r="123">
+      <c r="G123" s="7"/>
+    </row>
+    <row r="124">
+      <c r="G124" s="7"/>
+    </row>
+    <row r="125">
+      <c r="G125" s="7"/>
+    </row>
+    <row r="126">
+      <c r="G126" s="7"/>
+    </row>
+    <row r="127">
+      <c r="G127" s="7"/>
+    </row>
+    <row r="128">
+      <c r="G128" s="7"/>
+    </row>
+    <row r="129">
+      <c r="G129" s="7"/>
+    </row>
+    <row r="130">
+      <c r="G130" s="7"/>
+    </row>
+    <row r="131">
+      <c r="G131" s="7"/>
+    </row>
+    <row r="132">
+      <c r="G132" s="7"/>
+    </row>
+    <row r="133">
+      <c r="G133" s="7"/>
+    </row>
+    <row r="134">
+      <c r="G134" s="7"/>
+    </row>
+    <row r="135">
+      <c r="G135" s="7"/>
+    </row>
+    <row r="136">
+      <c r="G136" s="7"/>
+    </row>
+    <row r="137">
+      <c r="G137" s="7"/>
+    </row>
+    <row r="138">
+      <c r="G138" s="7"/>
+    </row>
+    <row r="139">
+      <c r="G139" s="7"/>
+    </row>
+    <row r="140">
+      <c r="G140" s="7"/>
+    </row>
+    <row r="141">
+      <c r="G141" s="7"/>
+    </row>
+    <row r="142">
+      <c r="G142" s="7"/>
+    </row>
+    <row r="143">
+      <c r="G143" s="7"/>
+    </row>
+    <row r="144">
+      <c r="G144" s="7"/>
+    </row>
+    <row r="145">
+      <c r="G145" s="7"/>
+    </row>
+    <row r="146">
+      <c r="G146" s="7"/>
+    </row>
+    <row r="147">
+      <c r="G147" s="7"/>
+    </row>
+    <row r="148">
+      <c r="G148" s="7"/>
+    </row>
+    <row r="149">
+      <c r="G149" s="7"/>
+    </row>
+    <row r="150">
+      <c r="G150" s="7"/>
+    </row>
+    <row r="151">
+      <c r="G151" s="7"/>
+    </row>
+    <row r="152">
+      <c r="G152" s="7"/>
+    </row>
+    <row r="153">
+      <c r="G153" s="7"/>
+    </row>
+    <row r="154">
+      <c r="G154" s="7"/>
+    </row>
+    <row r="155">
+      <c r="G155" s="7"/>
+    </row>
+    <row r="156">
+      <c r="G156" s="7"/>
+    </row>
+    <row r="157">
+      <c r="G157" s="7"/>
+    </row>
+    <row r="158">
+      <c r="G158" s="7"/>
+    </row>
+    <row r="159">
+      <c r="G159" s="7"/>
+    </row>
+    <row r="160">
+      <c r="G160" s="7"/>
+    </row>
+    <row r="161">
+      <c r="G161" s="7"/>
+    </row>
+    <row r="162">
+      <c r="G162" s="7"/>
+    </row>
+    <row r="163">
+      <c r="G163" s="7"/>
+    </row>
+    <row r="164">
+      <c r="G164" s="7"/>
+    </row>
+    <row r="165">
+      <c r="G165" s="7"/>
+    </row>
+    <row r="166">
+      <c r="G166" s="7"/>
+    </row>
+    <row r="167">
+      <c r="G167" s="7"/>
+    </row>
+    <row r="168">
+      <c r="G168" s="7"/>
+    </row>
+    <row r="169">
+      <c r="G169" s="7"/>
+    </row>
+    <row r="170">
+      <c r="G170" s="7"/>
+    </row>
+    <row r="171">
+      <c r="G171" s="7"/>
+    </row>
+    <row r="172">
+      <c r="G172" s="7"/>
+    </row>
+    <row r="173">
+      <c r="G173" s="7"/>
+    </row>
+    <row r="174">
+      <c r="G174" s="7"/>
+    </row>
+    <row r="175">
+      <c r="G175" s="7"/>
+    </row>
+    <row r="176">
+      <c r="G176" s="7"/>
+    </row>
+    <row r="177">
+      <c r="G177" s="7"/>
+    </row>
+    <row r="178">
+      <c r="G178" s="7"/>
+    </row>
+    <row r="179">
+      <c r="G179" s="7"/>
+    </row>
+    <row r="180">
+      <c r="G180" s="7"/>
+    </row>
+    <row r="181">
+      <c r="G181" s="7"/>
+    </row>
+    <row r="182">
+      <c r="G182" s="7"/>
+    </row>
+    <row r="183">
+      <c r="G183" s="7"/>
+    </row>
+    <row r="184">
+      <c r="G184" s="7"/>
+    </row>
+    <row r="185">
+      <c r="G185" s="7"/>
+    </row>
+    <row r="186">
+      <c r="G186" s="7"/>
+    </row>
+    <row r="187">
+      <c r="G187" s="7"/>
+    </row>
+    <row r="188">
+      <c r="G188" s="7"/>
+    </row>
+    <row r="189">
+      <c r="G189" s="7"/>
+    </row>
+    <row r="190">
+      <c r="G190" s="7"/>
+    </row>
+    <row r="191">
+      <c r="G191" s="7"/>
+    </row>
+    <row r="192">
+      <c r="G192" s="7"/>
+    </row>
+    <row r="193">
+      <c r="G193" s="7"/>
+    </row>
+    <row r="194">
+      <c r="G194" s="7"/>
+    </row>
+    <row r="195">
+      <c r="G195" s="7"/>
+    </row>
+    <row r="196">
+      <c r="G196" s="7"/>
+    </row>
+    <row r="197">
+      <c r="G197" s="7"/>
+    </row>
+    <row r="198">
+      <c r="G198" s="7"/>
+    </row>
+    <row r="199">
+      <c r="G199" s="7"/>
+    </row>
+    <row r="200">
+      <c r="G200" s="7"/>
+    </row>
+    <row r="201">
+      <c r="G201" s="7"/>
+    </row>
+    <row r="202">
+      <c r="G202" s="7"/>
+    </row>
+    <row r="203">
+      <c r="G203" s="7"/>
+    </row>
+    <row r="204">
+      <c r="G204" s="7"/>
+    </row>
+    <row r="205">
+      <c r="G205" s="7"/>
+    </row>
+    <row r="206">
+      <c r="G206" s="7"/>
+    </row>
+    <row r="207">
+      <c r="G207" s="7"/>
+    </row>
+    <row r="208">
+      <c r="G208" s="7"/>
+    </row>
+    <row r="209">
+      <c r="G209" s="7"/>
+    </row>
+    <row r="210">
+      <c r="G210" s="7"/>
+    </row>
+    <row r="211">
+      <c r="G211" s="7"/>
+    </row>
+    <row r="212">
+      <c r="G212" s="7"/>
+    </row>
+    <row r="213">
+      <c r="G213" s="7"/>
+    </row>
+    <row r="214">
+      <c r="G214" s="7"/>
+    </row>
+    <row r="215">
+      <c r="G215" s="7"/>
+    </row>
+    <row r="216">
+      <c r="G216" s="7"/>
+    </row>
+    <row r="217">
+      <c r="G217" s="7"/>
+    </row>
+    <row r="218">
+      <c r="G218" s="7"/>
+    </row>
+    <row r="219">
+      <c r="G219" s="7"/>
+    </row>
+    <row r="220">
+      <c r="G220" s="7"/>
+    </row>
+    <row r="221">
+      <c r="G221" s="7"/>
+    </row>
+    <row r="222">
+      <c r="G222" s="7"/>
+    </row>
+    <row r="223">
+      <c r="G223" s="7"/>
+    </row>
+    <row r="224">
+      <c r="G224" s="7"/>
+    </row>
+    <row r="225">
+      <c r="G225" s="7"/>
+    </row>
+    <row r="226">
+      <c r="G226" s="7"/>
+    </row>
+    <row r="227">
+      <c r="G227" s="7"/>
+    </row>
+    <row r="228">
+      <c r="G228" s="7"/>
+    </row>
+    <row r="229">
+      <c r="G229" s="7"/>
+    </row>
+    <row r="230">
+      <c r="G230" s="7"/>
+    </row>
+    <row r="231">
+      <c r="G231" s="7"/>
+    </row>
+    <row r="232">
+      <c r="G232" s="7"/>
+    </row>
+    <row r="233">
+      <c r="G233" s="7"/>
+    </row>
+    <row r="234">
+      <c r="G234" s="7"/>
+    </row>
+    <row r="235">
+      <c r="G235" s="7"/>
+    </row>
+    <row r="236">
+      <c r="G236" s="7"/>
+    </row>
+    <row r="237">
+      <c r="G237" s="7"/>
+    </row>
+    <row r="238">
+      <c r="G238" s="7"/>
+    </row>
+    <row r="239">
+      <c r="G239" s="7"/>
+    </row>
+    <row r="240">
+      <c r="G240" s="7"/>
+    </row>
+    <row r="241">
+      <c r="G241" s="7"/>
+    </row>
+    <row r="242">
+      <c r="G242" s="7"/>
+    </row>
+    <row r="243">
+      <c r="G243" s="7"/>
+    </row>
+    <row r="244">
+      <c r="G244" s="7"/>
+    </row>
+    <row r="245">
+      <c r="G245" s="7"/>
+    </row>
+    <row r="246">
+      <c r="G246" s="7"/>
+    </row>
+    <row r="247">
+      <c r="G247" s="7"/>
+    </row>
+    <row r="248">
+      <c r="G248" s="7"/>
+    </row>
+    <row r="249">
+      <c r="G249" s="7"/>
+    </row>
+    <row r="250">
+      <c r="G250" s="7"/>
+    </row>
+    <row r="251">
+      <c r="G251" s="7"/>
+    </row>
+    <row r="252">
+      <c r="G252" s="7"/>
+    </row>
+    <row r="253">
+      <c r="G253" s="7"/>
+    </row>
+    <row r="254">
+      <c r="G254" s="7"/>
+    </row>
+    <row r="255">
+      <c r="G255" s="7"/>
+    </row>
+    <row r="256">
+      <c r="G256" s="7"/>
+    </row>
+    <row r="257">
+      <c r="G257" s="7"/>
+    </row>
+    <row r="258">
+      <c r="G258" s="7"/>
+    </row>
+    <row r="259">
+      <c r="G259" s="7"/>
+    </row>
+    <row r="260">
+      <c r="G260" s="7"/>
+    </row>
+    <row r="261">
+      <c r="G261" s="7"/>
+    </row>
+    <row r="262">
+      <c r="G262" s="7"/>
+    </row>
+    <row r="263">
+      <c r="G263" s="7"/>
+    </row>
+    <row r="264">
+      <c r="G264" s="7"/>
+    </row>
+    <row r="265">
+      <c r="G265" s="7"/>
+    </row>
+    <row r="266">
+      <c r="G266" s="7"/>
+    </row>
+    <row r="267">
+      <c r="G267" s="7"/>
+    </row>
+    <row r="268">
+      <c r="G268" s="7"/>
+    </row>
+    <row r="269">
+      <c r="G269" s="7"/>
+    </row>
+    <row r="270">
+      <c r="G270" s="7"/>
+    </row>
+    <row r="271">
+      <c r="G271" s="7"/>
+    </row>
+    <row r="272">
+      <c r="G272" s="7"/>
+    </row>
+    <row r="273">
+      <c r="G273" s="7"/>
+    </row>
+    <row r="274">
+      <c r="G274" s="7"/>
+    </row>
+    <row r="275">
+      <c r="G275" s="7"/>
+    </row>
+    <row r="276">
+      <c r="G276" s="7"/>
+    </row>
+    <row r="277">
+      <c r="G277" s="7"/>
+    </row>
+    <row r="278">
+      <c r="G278" s="7"/>
+    </row>
+    <row r="279">
+      <c r="G279" s="7"/>
+    </row>
+    <row r="280">
+      <c r="G280" s="7"/>
+    </row>
+    <row r="281">
+      <c r="G281" s="7"/>
+    </row>
+    <row r="282">
+      <c r="G282" s="7"/>
+    </row>
+    <row r="283">
+      <c r="G283" s="7"/>
+    </row>
+    <row r="284">
+      <c r="G284" s="7"/>
+    </row>
+    <row r="285">
+      <c r="G285" s="7"/>
+    </row>
+    <row r="286">
+      <c r="G286" s="7"/>
+    </row>
+    <row r="287">
+      <c r="G287" s="7"/>
+    </row>
+    <row r="288">
+      <c r="G288" s="7"/>
+    </row>
+    <row r="289">
+      <c r="G289" s="7"/>
+    </row>
+    <row r="290">
+      <c r="G290" s="7"/>
+    </row>
+    <row r="291">
+      <c r="G291" s="7"/>
+    </row>
+    <row r="292">
+      <c r="G292" s="7"/>
+    </row>
+    <row r="293">
+      <c r="G293" s="7"/>
+    </row>
+    <row r="294">
+      <c r="G294" s="7"/>
+    </row>
+    <row r="295">
+      <c r="G295" s="7"/>
+    </row>
+    <row r="296">
+      <c r="G296" s="7"/>
+    </row>
+    <row r="297">
+      <c r="G297" s="7"/>
+    </row>
+    <row r="298">
+      <c r="G298" s="7"/>
+    </row>
+    <row r="299">
+      <c r="G299" s="7"/>
+    </row>
+    <row r="300">
+      <c r="G300" s="7"/>
+    </row>
+    <row r="301">
+      <c r="G301" s="7"/>
+    </row>
+    <row r="302">
+      <c r="G302" s="7"/>
+    </row>
+    <row r="303">
+      <c r="G303" s="7"/>
+    </row>
+    <row r="304">
+      <c r="G304" s="7"/>
+    </row>
+    <row r="305">
+      <c r="G305" s="7"/>
+    </row>
+    <row r="306">
+      <c r="G306" s="7"/>
+    </row>
+    <row r="307">
+      <c r="G307" s="7"/>
+    </row>
+    <row r="308">
+      <c r="G308" s="7"/>
+    </row>
+    <row r="309">
+      <c r="G309" s="7"/>
+    </row>
+    <row r="310">
+      <c r="G310" s="7"/>
+    </row>
+    <row r="311">
+      <c r="G311" s="7"/>
+    </row>
+    <row r="312">
+      <c r="G312" s="7"/>
+    </row>
+    <row r="313">
+      <c r="G313" s="7"/>
+    </row>
+    <row r="314">
+      <c r="G314" s="7"/>
+    </row>
+    <row r="315">
+      <c r="G315" s="7"/>
+    </row>
+    <row r="316">
+      <c r="G316" s="7"/>
+    </row>
+    <row r="317">
+      <c r="G317" s="7"/>
+    </row>
+    <row r="318">
+      <c r="G318" s="7"/>
+    </row>
+    <row r="319">
+      <c r="G319" s="7"/>
+    </row>
+    <row r="320">
+      <c r="G320" s="7"/>
+    </row>
+    <row r="321">
+      <c r="G321" s="7"/>
+    </row>
+    <row r="322">
+      <c r="G322" s="7"/>
+    </row>
+    <row r="323">
+      <c r="G323" s="7"/>
+    </row>
+    <row r="324">
+      <c r="G324" s="7"/>
+    </row>
+    <row r="325">
+      <c r="G325" s="7"/>
+    </row>
+    <row r="326">
+      <c r="G326" s="7"/>
+    </row>
+    <row r="327">
+      <c r="G327" s="7"/>
+    </row>
+    <row r="328">
+      <c r="G328" s="7"/>
+    </row>
+    <row r="329">
+      <c r="G329" s="7"/>
+    </row>
+    <row r="330">
+      <c r="G330" s="7"/>
+    </row>
+    <row r="331">
+      <c r="G331" s="7"/>
+    </row>
+    <row r="332">
+      <c r="G332" s="7"/>
+    </row>
+    <row r="333">
+      <c r="G333" s="7"/>
+    </row>
+    <row r="334">
+      <c r="G334" s="7"/>
+    </row>
+    <row r="335">
+      <c r="G335" s="7"/>
+    </row>
+    <row r="336">
+      <c r="G336" s="7"/>
+    </row>
+    <row r="337">
+      <c r="G337" s="7"/>
+    </row>
+    <row r="338">
+      <c r="G338" s="7"/>
+    </row>
+    <row r="339">
+      <c r="G339" s="7"/>
+    </row>
+    <row r="340">
+      <c r="G340" s="7"/>
+    </row>
+    <row r="341">
+      <c r="G341" s="7"/>
+    </row>
+    <row r="342">
+      <c r="G342" s="7"/>
+    </row>
+    <row r="343">
+      <c r="G343" s="7"/>
+    </row>
+    <row r="344">
+      <c r="G344" s="7"/>
+    </row>
+    <row r="345">
+      <c r="G345" s="7"/>
+    </row>
+    <row r="346">
+      <c r="G346" s="7"/>
+    </row>
+    <row r="347">
+      <c r="G347" s="7"/>
+    </row>
+    <row r="348">
+      <c r="G348" s="7"/>
+    </row>
+    <row r="349">
+      <c r="G349" s="7"/>
+    </row>
+    <row r="350">
+      <c r="G350" s="7"/>
+    </row>
+    <row r="351">
+      <c r="G351" s="7"/>
+    </row>
+    <row r="352">
+      <c r="G352" s="7"/>
+    </row>
+    <row r="353">
+      <c r="G353" s="7"/>
+    </row>
+    <row r="354">
+      <c r="G354" s="7"/>
+    </row>
+    <row r="355">
+      <c r="G355" s="7"/>
+    </row>
+    <row r="356">
+      <c r="G356" s="7"/>
+    </row>
+    <row r="357">
+      <c r="G357" s="7"/>
+    </row>
+    <row r="358">
+      <c r="G358" s="7"/>
+    </row>
+    <row r="359">
+      <c r="G359" s="7"/>
+    </row>
+    <row r="360">
+      <c r="G360" s="7"/>
+    </row>
+    <row r="361">
+      <c r="G361" s="7"/>
+    </row>
+    <row r="362">
+      <c r="G362" s="7"/>
+    </row>
+    <row r="363">
+      <c r="G363" s="7"/>
+    </row>
+    <row r="364">
+      <c r="G364" s="7"/>
+    </row>
+    <row r="365">
+      <c r="G365" s="7"/>
+    </row>
+    <row r="366">
+      <c r="G366" s="7"/>
+    </row>
+    <row r="367">
+      <c r="G367" s="7"/>
+    </row>
+    <row r="368">
+      <c r="G368" s="7"/>
+    </row>
+    <row r="369">
+      <c r="G369" s="7"/>
+    </row>
+    <row r="370">
+      <c r="G370" s="7"/>
+    </row>
+    <row r="371">
+      <c r="G371" s="7"/>
+    </row>
+    <row r="372">
+      <c r="G372" s="7"/>
+    </row>
+    <row r="373">
+      <c r="G373" s="7"/>
+    </row>
+    <row r="374">
+      <c r="G374" s="7"/>
+    </row>
+    <row r="375">
+      <c r="G375" s="7"/>
+    </row>
+    <row r="376">
+      <c r="G376" s="7"/>
+    </row>
+    <row r="377">
+      <c r="G377" s="7"/>
+    </row>
+    <row r="378">
+      <c r="G378" s="7"/>
+    </row>
+    <row r="379">
+      <c r="G379" s="7"/>
+    </row>
+    <row r="380">
+      <c r="G380" s="7"/>
+    </row>
+    <row r="381">
+      <c r="G381" s="7"/>
+    </row>
+    <row r="382">
+      <c r="G382" s="7"/>
+    </row>
+    <row r="383">
+      <c r="G383" s="7"/>
+    </row>
+    <row r="384">
+      <c r="G384" s="7"/>
+    </row>
+    <row r="385">
+      <c r="G385" s="7"/>
+    </row>
+    <row r="386">
+      <c r="G386" s="7"/>
+    </row>
+    <row r="387">
+      <c r="G387" s="7"/>
+    </row>
+    <row r="388">
+      <c r="G388" s="7"/>
+    </row>
+    <row r="389">
+      <c r="G389" s="7"/>
+    </row>
+    <row r="390">
+      <c r="G390" s="7"/>
+    </row>
+    <row r="391">
+      <c r="G391" s="7"/>
+    </row>
+    <row r="392">
+      <c r="G392" s="7"/>
+    </row>
+    <row r="393">
+      <c r="G393" s="7"/>
+    </row>
+    <row r="394">
+      <c r="G394" s="7"/>
+    </row>
+    <row r="395">
+      <c r="G395" s="7"/>
+    </row>
+    <row r="396">
+      <c r="G396" s="7"/>
+    </row>
+    <row r="397">
+      <c r="G397" s="7"/>
+    </row>
+    <row r="398">
+      <c r="G398" s="7"/>
+    </row>
+    <row r="399">
+      <c r="G399" s="7"/>
+    </row>
+    <row r="400">
+      <c r="G400" s="7"/>
+    </row>
+    <row r="401">
+      <c r="G401" s="7"/>
+    </row>
+    <row r="402">
+      <c r="G402" s="7"/>
+    </row>
+    <row r="403">
+      <c r="G403" s="7"/>
+    </row>
+    <row r="404">
+      <c r="G404" s="7"/>
+    </row>
+    <row r="405">
+      <c r="G405" s="7"/>
+    </row>
+    <row r="406">
+      <c r="G406" s="7"/>
+    </row>
+    <row r="407">
+      <c r="G407" s="7"/>
+    </row>
+    <row r="408">
+      <c r="G408" s="7"/>
+    </row>
+    <row r="409">
+      <c r="G409" s="7"/>
+    </row>
+    <row r="410">
+      <c r="G410" s="7"/>
+    </row>
+    <row r="411">
+      <c r="G411" s="7"/>
+    </row>
+    <row r="412">
+      <c r="G412" s="7"/>
+    </row>
+    <row r="413">
+      <c r="G413" s="7"/>
+    </row>
+    <row r="414">
+      <c r="G414" s="7"/>
+    </row>
+    <row r="415">
+      <c r="G415" s="7"/>
+    </row>
+    <row r="416">
+      <c r="G416" s="7"/>
+    </row>
+    <row r="417">
+      <c r="G417" s="7"/>
+    </row>
+    <row r="418">
+      <c r="G418" s="7"/>
+    </row>
+    <row r="419">
+      <c r="G419" s="7"/>
+    </row>
+    <row r="420">
+      <c r="G420" s="7"/>
+    </row>
+    <row r="421">
+      <c r="G421" s="7"/>
+    </row>
+    <row r="422">
+      <c r="G422" s="7"/>
+    </row>
+    <row r="423">
+      <c r="G423" s="7"/>
+    </row>
+    <row r="424">
+      <c r="G424" s="7"/>
+    </row>
+    <row r="425">
+      <c r="G425" s="7"/>
+    </row>
+    <row r="426">
+      <c r="G426" s="7"/>
+    </row>
+    <row r="427">
+      <c r="G427" s="7"/>
+    </row>
+    <row r="428">
+      <c r="G428" s="7"/>
+    </row>
+    <row r="429">
+      <c r="G429" s="7"/>
+    </row>
+    <row r="430">
+      <c r="G430" s="7"/>
+    </row>
+    <row r="431">
+      <c r="G431" s="7"/>
+    </row>
+    <row r="432">
+      <c r="G432" s="7"/>
+    </row>
+    <row r="433">
+      <c r="G433" s="7"/>
+    </row>
+    <row r="434">
+      <c r="G434" s="7"/>
+    </row>
+    <row r="435">
+      <c r="G435" s="7"/>
+    </row>
+    <row r="436">
+      <c r="G436" s="7"/>
+    </row>
+    <row r="437">
+      <c r="G437" s="7"/>
+    </row>
+    <row r="438">
+      <c r="G438" s="7"/>
+    </row>
+    <row r="439">
+      <c r="G439" s="7"/>
+    </row>
+    <row r="440">
+      <c r="G440" s="7"/>
+    </row>
+    <row r="441">
+      <c r="G441" s="7"/>
+    </row>
+    <row r="442">
+      <c r="G442" s="7"/>
+    </row>
+    <row r="443">
+      <c r="G443" s="7"/>
+    </row>
+    <row r="444">
+      <c r="G444" s="7"/>
+    </row>
+    <row r="445">
+      <c r="G445" s="7"/>
+    </row>
+    <row r="446">
+      <c r="G446" s="7"/>
+    </row>
+    <row r="447">
+      <c r="G447" s="7"/>
+    </row>
+    <row r="448">
+      <c r="G448" s="7"/>
+    </row>
+    <row r="449">
+      <c r="G449" s="7"/>
+    </row>
+    <row r="450">
+      <c r="G450" s="7"/>
+    </row>
+    <row r="451">
+      <c r="G451" s="7"/>
+    </row>
+    <row r="452">
+      <c r="G452" s="7"/>
+    </row>
+    <row r="453">
+      <c r="G453" s="7"/>
+    </row>
+    <row r="454">
+      <c r="G454" s="7"/>
+    </row>
+    <row r="455">
+      <c r="G455" s="7"/>
+    </row>
+    <row r="456">
+      <c r="G456" s="7"/>
+    </row>
+    <row r="457">
+      <c r="G457" s="7"/>
+    </row>
+    <row r="458">
+      <c r="G458" s="7"/>
+    </row>
+    <row r="459">
+      <c r="G459" s="7"/>
+    </row>
+    <row r="460">
+      <c r="G460" s="7"/>
+    </row>
+    <row r="461">
+      <c r="G461" s="7"/>
+    </row>
+    <row r="462">
+      <c r="G462" s="7"/>
+    </row>
+    <row r="463">
+      <c r="G463" s="7"/>
+    </row>
+    <row r="464">
+      <c r="G464" s="7"/>
+    </row>
+    <row r="465">
+      <c r="G465" s="7"/>
+    </row>
+    <row r="466">
+      <c r="G466" s="7"/>
+    </row>
+    <row r="467">
+      <c r="G467" s="7"/>
+    </row>
+    <row r="468">
+      <c r="G468" s="7"/>
+    </row>
+    <row r="469">
+      <c r="G469" s="7"/>
+    </row>
+    <row r="470">
+      <c r="G470" s="7"/>
+    </row>
+    <row r="471">
+      <c r="G471" s="7"/>
+    </row>
+    <row r="472">
+      <c r="G472" s="7"/>
+    </row>
+    <row r="473">
+      <c r="G473" s="7"/>
+    </row>
+    <row r="474">
+      <c r="G474" s="7"/>
+    </row>
+    <row r="475">
+      <c r="G475" s="7"/>
+    </row>
+    <row r="476">
+      <c r="G476" s="7"/>
+    </row>
+    <row r="477">
+      <c r="G477" s="7"/>
+    </row>
+    <row r="478">
+      <c r="G478" s="7"/>
+    </row>
+    <row r="479">
+      <c r="G479" s="7"/>
+    </row>
+    <row r="480">
+      <c r="G480" s="7"/>
+    </row>
+    <row r="481">
+      <c r="G481" s="7"/>
+    </row>
+    <row r="482">
+      <c r="G482" s="7"/>
+    </row>
+    <row r="483">
+      <c r="G483" s="7"/>
+    </row>
+    <row r="484">
+      <c r="G484" s="7"/>
+    </row>
+    <row r="485">
+      <c r="G485" s="7"/>
+    </row>
+    <row r="486">
+      <c r="G486" s="7"/>
+    </row>
+    <row r="487">
+      <c r="G487" s="7"/>
+    </row>
+    <row r="488">
+      <c r="G488" s="7"/>
+    </row>
+    <row r="489">
+      <c r="G489" s="7"/>
+    </row>
+    <row r="490">
+      <c r="G490" s="7"/>
+    </row>
+    <row r="491">
+      <c r="G491" s="7"/>
+    </row>
+    <row r="492">
+      <c r="G492" s="7"/>
+    </row>
+    <row r="493">
+      <c r="G493" s="7"/>
+    </row>
+    <row r="494">
+      <c r="G494" s="7"/>
+    </row>
+    <row r="495">
+      <c r="G495" s="7"/>
+    </row>
+    <row r="496">
+      <c r="G496" s="7"/>
+    </row>
+    <row r="497">
+      <c r="G497" s="7"/>
+    </row>
+    <row r="498">
+      <c r="G498" s="7"/>
+    </row>
+    <row r="499">
+      <c r="G499" s="7"/>
+    </row>
+    <row r="500">
+      <c r="G500" s="7"/>
+    </row>
+    <row r="501">
+      <c r="G501" s="7"/>
+    </row>
+    <row r="502">
+      <c r="G502" s="7"/>
+    </row>
+    <row r="503">
+      <c r="G503" s="7"/>
+    </row>
+    <row r="504">
+      <c r="G504" s="7"/>
+    </row>
+    <row r="505">
+      <c r="G505" s="7"/>
+    </row>
+    <row r="506">
+      <c r="G506" s="7"/>
+    </row>
+    <row r="507">
+      <c r="G507" s="7"/>
+    </row>
+    <row r="508">
+      <c r="G508" s="7"/>
+    </row>
+    <row r="509">
+      <c r="G509" s="7"/>
+    </row>
+    <row r="510">
+      <c r="G510" s="7"/>
+    </row>
+    <row r="511">
+      <c r="G511" s="7"/>
+    </row>
+    <row r="512">
+      <c r="G512" s="7"/>
+    </row>
+    <row r="513">
+      <c r="G513" s="7"/>
+    </row>
+    <row r="514">
+      <c r="G514" s="7"/>
+    </row>
+    <row r="515">
+      <c r="G515" s="7"/>
+    </row>
+    <row r="516">
+      <c r="G516" s="7"/>
+    </row>
+    <row r="517">
+      <c r="G517" s="7"/>
+    </row>
+    <row r="518">
+      <c r="G518" s="7"/>
+    </row>
+    <row r="519">
+      <c r="G519" s="7"/>
+    </row>
+    <row r="520">
+      <c r="G520" s="7"/>
+    </row>
+    <row r="521">
+      <c r="G521" s="7"/>
+    </row>
+    <row r="522">
+      <c r="G522" s="7"/>
+    </row>
+    <row r="523">
+      <c r="G523" s="7"/>
+    </row>
+    <row r="524">
+      <c r="G524" s="7"/>
+    </row>
+    <row r="525">
+      <c r="G525" s="7"/>
+    </row>
+    <row r="526">
+      <c r="G526" s="7"/>
+    </row>
+    <row r="527">
+      <c r="G527" s="7"/>
+    </row>
+    <row r="528">
+      <c r="G528" s="7"/>
+    </row>
+    <row r="529">
+      <c r="G529" s="7"/>
+    </row>
+    <row r="530">
+      <c r="G530" s="7"/>
+    </row>
+    <row r="531">
+      <c r="G531" s="7"/>
+    </row>
+    <row r="532">
+      <c r="G532" s="7"/>
+    </row>
+    <row r="533">
+      <c r="G533" s="7"/>
+    </row>
+    <row r="534">
+      <c r="G534" s="7"/>
+    </row>
+    <row r="535">
+      <c r="G535" s="7"/>
+    </row>
+    <row r="536">
+      <c r="G536" s="7"/>
+    </row>
+    <row r="537">
+      <c r="G537" s="7"/>
+    </row>
+    <row r="538">
+      <c r="G538" s="7"/>
+    </row>
+    <row r="539">
+      <c r="G539" s="7"/>
+    </row>
+    <row r="540">
+      <c r="G540" s="7"/>
+    </row>
+    <row r="541">
+      <c r="G541" s="7"/>
+    </row>
+    <row r="542">
+      <c r="G542" s="7"/>
+    </row>
+    <row r="543">
+      <c r="G543" s="7"/>
+    </row>
+    <row r="544">
+      <c r="G544" s="7"/>
+    </row>
+    <row r="545">
+      <c r="G545" s="7"/>
+    </row>
+    <row r="546">
+      <c r="G546" s="7"/>
+    </row>
+    <row r="547">
+      <c r="G547" s="7"/>
+    </row>
+    <row r="548">
+      <c r="G548" s="7"/>
+    </row>
+    <row r="549">
+      <c r="G549" s="7"/>
+    </row>
+    <row r="550">
+      <c r="G550" s="7"/>
+    </row>
+    <row r="551">
+      <c r="G551" s="7"/>
+    </row>
+    <row r="552">
+      <c r="G552" s="7"/>
+    </row>
+    <row r="553">
+      <c r="G553" s="7"/>
+    </row>
+    <row r="554">
+      <c r="G554" s="7"/>
+    </row>
+    <row r="555">
+      <c r="G555" s="7"/>
+    </row>
+    <row r="556">
+      <c r="G556" s="7"/>
+    </row>
+    <row r="557">
+      <c r="G557" s="7"/>
+    </row>
+    <row r="558">
+      <c r="G558" s="7"/>
+    </row>
+    <row r="559">
+      <c r="G559" s="7"/>
+    </row>
+    <row r="560">
+      <c r="G560" s="7"/>
+    </row>
+    <row r="561">
+      <c r="G561" s="7"/>
+    </row>
+    <row r="562">
+      <c r="G562" s="7"/>
+    </row>
+    <row r="563">
+      <c r="G563" s="7"/>
+    </row>
+    <row r="564">
+      <c r="G564" s="7"/>
+    </row>
+    <row r="565">
+      <c r="G565" s="7"/>
+    </row>
+    <row r="566">
+      <c r="G566" s="7"/>
+    </row>
+    <row r="567">
+      <c r="G567" s="7"/>
+    </row>
+    <row r="568">
+      <c r="G568" s="7"/>
+    </row>
+    <row r="569">
+      <c r="G569" s="7"/>
+    </row>
+    <row r="570">
+      <c r="G570" s="7"/>
+    </row>
+    <row r="571">
+      <c r="G571" s="7"/>
+    </row>
+    <row r="572">
+      <c r="G572" s="7"/>
+    </row>
+    <row r="573">
+      <c r="G573" s="7"/>
+    </row>
+    <row r="574">
+      <c r="G574" s="7"/>
+    </row>
+    <row r="575">
+      <c r="G575" s="7"/>
+    </row>
+    <row r="576">
+      <c r="G576" s="7"/>
+    </row>
+    <row r="577">
+      <c r="G577" s="7"/>
+    </row>
+    <row r="578">
+      <c r="G578" s="7"/>
+    </row>
+    <row r="579">
+      <c r="G579" s="7"/>
+    </row>
+    <row r="580">
+      <c r="G580" s="7"/>
+    </row>
+    <row r="581">
+      <c r="G581" s="7"/>
+    </row>
+    <row r="582">
+      <c r="G582" s="7"/>
+    </row>
+    <row r="583">
+      <c r="G583" s="7"/>
+    </row>
+    <row r="584">
+      <c r="G584" s="7"/>
+    </row>
+    <row r="585">
+      <c r="G585" s="7"/>
+    </row>
+    <row r="586">
+      <c r="G586" s="7"/>
+    </row>
+    <row r="587">
+      <c r="G587" s="7"/>
+    </row>
+    <row r="588">
+      <c r="G588" s="7"/>
+    </row>
+    <row r="589">
+      <c r="G589" s="7"/>
+    </row>
+    <row r="590">
+      <c r="G590" s="7"/>
+    </row>
+    <row r="591">
+      <c r="G591" s="7"/>
+    </row>
+    <row r="592">
+      <c r="G592" s="7"/>
+    </row>
+    <row r="593">
+      <c r="G593" s="7"/>
+    </row>
+    <row r="594">
+      <c r="G594" s="7"/>
+    </row>
+    <row r="595">
+      <c r="G595" s="7"/>
+    </row>
+    <row r="596">
+      <c r="G596" s="7"/>
+    </row>
+    <row r="597">
+      <c r="G597" s="7"/>
+    </row>
+    <row r="598">
+      <c r="G598" s="7"/>
+    </row>
+    <row r="599">
+      <c r="G599" s="7"/>
+    </row>
+    <row r="600">
+      <c r="G600" s="7"/>
+    </row>
+    <row r="601">
+      <c r="G601" s="7"/>
+    </row>
+    <row r="602">
+      <c r="G602" s="7"/>
+    </row>
+    <row r="603">
+      <c r="G603" s="7"/>
+    </row>
+    <row r="604">
+      <c r="G604" s="7"/>
+    </row>
+    <row r="605">
+      <c r="G605" s="7"/>
+    </row>
+    <row r="606">
+      <c r="G606" s="7"/>
+    </row>
+    <row r="607">
+      <c r="G607" s="7"/>
+    </row>
+    <row r="608">
+      <c r="G608" s="7"/>
+    </row>
+    <row r="609">
+      <c r="G609" s="7"/>
+    </row>
+    <row r="610">
+      <c r="G610" s="7"/>
+    </row>
+    <row r="611">
+      <c r="G611" s="7"/>
+    </row>
+    <row r="612">
+      <c r="G612" s="7"/>
+    </row>
+    <row r="613">
+      <c r="G613" s="7"/>
+    </row>
+    <row r="614">
+      <c r="G614" s="7"/>
+    </row>
+    <row r="615">
+      <c r="G615" s="7"/>
+    </row>
+    <row r="616">
+      <c r="G616" s="7"/>
+    </row>
+    <row r="617">
+      <c r="G617" s="7"/>
+    </row>
+    <row r="618">
+      <c r="G618" s="7"/>
+    </row>
+    <row r="619">
+      <c r="G619" s="7"/>
+    </row>
+    <row r="620">
+      <c r="G620" s="7"/>
+    </row>
+    <row r="621">
+      <c r="G621" s="7"/>
+    </row>
+    <row r="622">
+      <c r="G622" s="7"/>
+    </row>
+    <row r="623">
+      <c r="G623" s="7"/>
+    </row>
+    <row r="624">
+      <c r="G624" s="7"/>
+    </row>
+    <row r="625">
+      <c r="G625" s="7"/>
+    </row>
+    <row r="626">
+      <c r="G626" s="7"/>
+    </row>
+    <row r="627">
+      <c r="G627" s="7"/>
+    </row>
+    <row r="628">
+      <c r="G628" s="7"/>
+    </row>
+    <row r="629">
+      <c r="G629" s="7"/>
+    </row>
+    <row r="630">
+      <c r="G630" s="7"/>
+    </row>
+    <row r="631">
+      <c r="G631" s="7"/>
+    </row>
+    <row r="632">
+      <c r="G632" s="7"/>
+    </row>
+    <row r="633">
+      <c r="G633" s="7"/>
+    </row>
+    <row r="634">
+      <c r="G634" s="7"/>
+    </row>
+    <row r="635">
+      <c r="G635" s="7"/>
+    </row>
+    <row r="636">
+      <c r="G636" s="7"/>
+    </row>
+    <row r="637">
+      <c r="G637" s="7"/>
+    </row>
+    <row r="638">
+      <c r="G638" s="7"/>
+    </row>
+    <row r="639">
+      <c r="G639" s="7"/>
+    </row>
+    <row r="640">
+      <c r="G640" s="7"/>
+    </row>
+    <row r="641">
+      <c r="G641" s="7"/>
+    </row>
+    <row r="642">
+      <c r="G642" s="7"/>
+    </row>
+    <row r="643">
+      <c r="G643" s="7"/>
+    </row>
+    <row r="644">
+      <c r="G644" s="7"/>
+    </row>
+    <row r="645">
+      <c r="G645" s="7"/>
+    </row>
+    <row r="646">
+      <c r="G646" s="7"/>
+    </row>
+    <row r="647">
+      <c r="G647" s="7"/>
+    </row>
+    <row r="648">
+      <c r="G648" s="7"/>
+    </row>
+    <row r="649">
+      <c r="G649" s="7"/>
+    </row>
+    <row r="650">
+      <c r="G650" s="7"/>
+    </row>
+    <row r="651">
+      <c r="G651" s="7"/>
+    </row>
+    <row r="652">
+      <c r="G652" s="7"/>
+    </row>
+    <row r="653">
+      <c r="G653" s="7"/>
+    </row>
+    <row r="654">
+      <c r="G654" s="7"/>
+    </row>
+    <row r="655">
+      <c r="G655" s="7"/>
+    </row>
+    <row r="656">
+      <c r="G656" s="7"/>
+    </row>
+    <row r="657">
+      <c r="G657" s="7"/>
+    </row>
+    <row r="658">
+      <c r="G658" s="7"/>
+    </row>
+    <row r="659">
+      <c r="G659" s="7"/>
+    </row>
+    <row r="660">
+      <c r="G660" s="7"/>
+    </row>
+    <row r="661">
+      <c r="G661" s="7"/>
+    </row>
+    <row r="662">
+      <c r="G662" s="7"/>
+    </row>
+    <row r="663">
+      <c r="G663" s="7"/>
+    </row>
+    <row r="664">
+      <c r="G664" s="7"/>
+    </row>
+    <row r="665">
+      <c r="G665" s="7"/>
+    </row>
+    <row r="666">
+      <c r="G666" s="7"/>
+    </row>
+    <row r="667">
+      <c r="G667" s="7"/>
+    </row>
+    <row r="668">
+      <c r="G668" s="7"/>
+    </row>
+    <row r="669">
+      <c r="G669" s="7"/>
+    </row>
+    <row r="670">
+      <c r="G670" s="7"/>
+    </row>
+    <row r="671">
+      <c r="G671" s="7"/>
+    </row>
+    <row r="672">
+      <c r="G672" s="7"/>
+    </row>
+    <row r="673">
+      <c r="G673" s="7"/>
+    </row>
+    <row r="674">
+      <c r="G674" s="7"/>
+    </row>
+    <row r="675">
+      <c r="G675" s="7"/>
+    </row>
+    <row r="676">
+      <c r="G676" s="7"/>
+    </row>
+    <row r="677">
+      <c r="G677" s="7"/>
+    </row>
+    <row r="678">
+      <c r="G678" s="7"/>
+    </row>
+    <row r="679">
+      <c r="G679" s="7"/>
+    </row>
+    <row r="680">
+      <c r="G680" s="7"/>
+    </row>
+    <row r="681">
+      <c r="G681" s="7"/>
+    </row>
+    <row r="682">
+      <c r="G682" s="7"/>
+    </row>
+    <row r="683">
+      <c r="G683" s="7"/>
+    </row>
+    <row r="684">
+      <c r="G684" s="7"/>
+    </row>
+    <row r="685">
+      <c r="G685" s="7"/>
+    </row>
+    <row r="686">
+      <c r="G686" s="7"/>
+    </row>
+    <row r="687">
+      <c r="G687" s="7"/>
+    </row>
+    <row r="688">
+      <c r="G688" s="7"/>
+    </row>
+    <row r="689">
+      <c r="G689" s="7"/>
+    </row>
+    <row r="690">
+      <c r="G690" s="7"/>
+    </row>
+    <row r="691">
+      <c r="G691" s="7"/>
+    </row>
+    <row r="692">
+      <c r="G692" s="7"/>
+    </row>
+    <row r="693">
+      <c r="G693" s="7"/>
+    </row>
+    <row r="694">
+      <c r="G694" s="7"/>
+    </row>
+    <row r="695">
+      <c r="G695" s="7"/>
+    </row>
+    <row r="696">
+      <c r="G696" s="7"/>
+    </row>
+    <row r="697">
+      <c r="G697" s="7"/>
+    </row>
+    <row r="698">
+      <c r="G698" s="7"/>
+    </row>
+    <row r="699">
+      <c r="G699" s="7"/>
+    </row>
+    <row r="700">
+      <c r="G700" s="7"/>
+    </row>
+    <row r="701">
+      <c r="G701" s="7"/>
+    </row>
+    <row r="702">
+      <c r="G702" s="7"/>
+    </row>
+    <row r="703">
+      <c r="G703" s="7"/>
+    </row>
+    <row r="704">
+      <c r="G704" s="7"/>
+    </row>
+    <row r="705">
+      <c r="G705" s="7"/>
+    </row>
+    <row r="706">
+      <c r="G706" s="7"/>
+    </row>
+    <row r="707">
+      <c r="G707" s="7"/>
+    </row>
+    <row r="708">
+      <c r="G708" s="7"/>
+    </row>
+    <row r="709">
+      <c r="G709" s="7"/>
+    </row>
+    <row r="710">
+      <c r="G710" s="7"/>
+    </row>
+    <row r="711">
+      <c r="G711" s="7"/>
+    </row>
+    <row r="712">
+      <c r="G712" s="7"/>
+    </row>
+    <row r="713">
+      <c r="G713" s="7"/>
+    </row>
+    <row r="714">
+      <c r="G714" s="7"/>
+    </row>
+    <row r="715">
+      <c r="G715" s="7"/>
+    </row>
+    <row r="716">
+      <c r="G716" s="7"/>
+    </row>
+    <row r="717">
+      <c r="G717" s="7"/>
+    </row>
+    <row r="718">
+      <c r="G718" s="7"/>
+    </row>
+    <row r="719">
+      <c r="G719" s="7"/>
+    </row>
+    <row r="720">
+      <c r="G720" s="7"/>
+    </row>
+    <row r="721">
+      <c r="G721" s="7"/>
+    </row>
+    <row r="722">
+      <c r="G722" s="7"/>
+    </row>
+    <row r="723">
+      <c r="G723" s="7"/>
+    </row>
+    <row r="724">
+      <c r="G724" s="7"/>
+    </row>
+    <row r="725">
+      <c r="G725" s="7"/>
+    </row>
+    <row r="726">
+      <c r="G726" s="7"/>
+    </row>
+    <row r="727">
+      <c r="G727" s="7"/>
+    </row>
+    <row r="728">
+      <c r="G728" s="7"/>
+    </row>
+    <row r="729">
+      <c r="G729" s="7"/>
+    </row>
+    <row r="730">
+      <c r="G730" s="7"/>
+    </row>
+    <row r="731">
+      <c r="G731" s="7"/>
+    </row>
+    <row r="732">
+      <c r="G732" s="7"/>
+    </row>
+    <row r="733">
+      <c r="G733" s="7"/>
+    </row>
+    <row r="734">
+      <c r="G734" s="7"/>
+    </row>
+    <row r="735">
+      <c r="G735" s="7"/>
+    </row>
+    <row r="736">
+      <c r="G736" s="7"/>
+    </row>
+    <row r="737">
+      <c r="G737" s="7"/>
+    </row>
+    <row r="738">
+      <c r="G738" s="7"/>
+    </row>
+    <row r="739">
+      <c r="G739" s="7"/>
+    </row>
+    <row r="740">
+      <c r="G740" s="7"/>
+    </row>
+    <row r="741">
+      <c r="G741" s="7"/>
+    </row>
+    <row r="742">
+      <c r="G742" s="7"/>
+    </row>
+    <row r="743">
+      <c r="G743" s="7"/>
+    </row>
+    <row r="744">
+      <c r="G744" s="7"/>
+    </row>
+    <row r="745">
+      <c r="G745" s="7"/>
+    </row>
+    <row r="746">
+      <c r="G746" s="7"/>
+    </row>
+    <row r="747">
+      <c r="G747" s="7"/>
+    </row>
+    <row r="748">
+      <c r="G748" s="7"/>
+    </row>
+    <row r="749">
+      <c r="G749" s="7"/>
+    </row>
+    <row r="750">
+      <c r="G750" s="7"/>
+    </row>
+    <row r="751">
+      <c r="G751" s="7"/>
+    </row>
+    <row r="752">
+      <c r="G752" s="7"/>
+    </row>
+    <row r="753">
+      <c r="G753" s="7"/>
+    </row>
+    <row r="754">
+      <c r="G754" s="7"/>
+    </row>
+    <row r="755">
+      <c r="G755" s="7"/>
+    </row>
+    <row r="756">
+      <c r="G756" s="7"/>
+    </row>
+    <row r="757">
+      <c r="G757" s="7"/>
+    </row>
+    <row r="758">
+      <c r="G758" s="7"/>
+    </row>
+    <row r="759">
+      <c r="G759" s="7"/>
+    </row>
+    <row r="760">
+      <c r="G760" s="7"/>
+    </row>
+    <row r="761">
+      <c r="G761" s="7"/>
+    </row>
+    <row r="762">
+      <c r="G762" s="7"/>
+    </row>
+    <row r="763">
+      <c r="G763" s="7"/>
+    </row>
+    <row r="764">
+      <c r="G764" s="7"/>
+    </row>
+    <row r="765">
+      <c r="G765" s="7"/>
+    </row>
+    <row r="766">
+      <c r="G766" s="7"/>
+    </row>
+    <row r="767">
+      <c r="G767" s="7"/>
+    </row>
+    <row r="768">
+      <c r="G768" s="7"/>
+    </row>
+    <row r="769">
+      <c r="G769" s="7"/>
+    </row>
+    <row r="770">
+      <c r="G770" s="7"/>
+    </row>
+    <row r="771">
+      <c r="G771" s="7"/>
+    </row>
+    <row r="772">
+      <c r="G772" s="7"/>
+    </row>
+    <row r="773">
+      <c r="G773" s="7"/>
+    </row>
+    <row r="774">
+      <c r="G774" s="7"/>
+    </row>
+    <row r="775">
+      <c r="G775" s="7"/>
+    </row>
+    <row r="776">
+      <c r="G776" s="7"/>
+    </row>
+    <row r="777">
+      <c r="G777" s="7"/>
+    </row>
+    <row r="778">
+      <c r="G778" s="7"/>
+    </row>
+    <row r="779">
+      <c r="G779" s="7"/>
+    </row>
+    <row r="780">
+      <c r="G780" s="7"/>
+    </row>
+    <row r="781">
+      <c r="G781" s="7"/>
+    </row>
+    <row r="782">
+      <c r="G782" s="7"/>
+    </row>
+    <row r="783">
+      <c r="G783" s="7"/>
+    </row>
+    <row r="784">
+      <c r="G784" s="7"/>
+    </row>
+    <row r="785">
+      <c r="G785" s="7"/>
+    </row>
+    <row r="786">
+      <c r="G786" s="7"/>
+    </row>
+    <row r="787">
+      <c r="G787" s="7"/>
+    </row>
+    <row r="788">
+      <c r="G788" s="7"/>
+    </row>
+    <row r="789">
+      <c r="G789" s="7"/>
+    </row>
+    <row r="790">
+      <c r="G790" s="7"/>
+    </row>
+    <row r="791">
+      <c r="G791" s="7"/>
+    </row>
+    <row r="792">
+      <c r="G792" s="7"/>
+    </row>
+    <row r="793">
+      <c r="G793" s="7"/>
+    </row>
+    <row r="794">
+      <c r="G794" s="7"/>
+    </row>
+    <row r="795">
+      <c r="G795" s="7"/>
+    </row>
+    <row r="796">
+      <c r="G796" s="7"/>
+    </row>
+    <row r="797">
+      <c r="G797" s="7"/>
+    </row>
+    <row r="798">
+      <c r="G798" s="7"/>
+    </row>
+    <row r="799">
+      <c r="G799" s="7"/>
+    </row>
+    <row r="800">
+      <c r="G800" s="7"/>
+    </row>
+    <row r="801">
+      <c r="G801" s="7"/>
+    </row>
+    <row r="802">
+      <c r="G802" s="7"/>
+    </row>
+    <row r="803">
+      <c r="G803" s="7"/>
+    </row>
+    <row r="804">
+      <c r="G804" s="7"/>
+    </row>
+    <row r="805">
+      <c r="G805" s="7"/>
+    </row>
+    <row r="806">
+      <c r="G806" s="7"/>
+    </row>
+    <row r="807">
+      <c r="G807" s="7"/>
+    </row>
+    <row r="808">
+      <c r="G808" s="7"/>
+    </row>
+    <row r="809">
+      <c r="G809" s="7"/>
+    </row>
+    <row r="810">
+      <c r="G810" s="7"/>
+    </row>
+    <row r="811">
+      <c r="G811" s="7"/>
+    </row>
+    <row r="812">
+      <c r="G812" s="7"/>
+    </row>
+    <row r="813">
+      <c r="G813" s="7"/>
+    </row>
+    <row r="814">
+      <c r="G814" s="7"/>
+    </row>
+    <row r="815">
+      <c r="G815" s="7"/>
+    </row>
+    <row r="816">
+      <c r="G816" s="7"/>
+    </row>
+    <row r="817">
+      <c r="G817" s="7"/>
+    </row>
+    <row r="818">
+      <c r="G818" s="7"/>
+    </row>
+    <row r="819">
+      <c r="G819" s="7"/>
+    </row>
+    <row r="820">
+      <c r="G820" s="7"/>
+    </row>
+    <row r="821">
+      <c r="G821" s="7"/>
+    </row>
+    <row r="822">
+      <c r="G822" s="7"/>
+    </row>
+    <row r="823">
+      <c r="G823" s="7"/>
+    </row>
+    <row r="824">
+      <c r="G824" s="7"/>
+    </row>
+    <row r="825">
+      <c r="G825" s="7"/>
+    </row>
+    <row r="826">
+      <c r="G826" s="7"/>
+    </row>
+    <row r="827">
+      <c r="G827" s="7"/>
+    </row>
+    <row r="828">
+      <c r="G828" s="7"/>
+    </row>
+    <row r="829">
+      <c r="G829" s="7"/>
+    </row>
+    <row r="830">
+      <c r="G830" s="7"/>
+    </row>
+    <row r="831">
+      <c r="G831" s="7"/>
+    </row>
+    <row r="832">
+      <c r="G832" s="7"/>
+    </row>
+    <row r="833">
+      <c r="G833" s="7"/>
+    </row>
+    <row r="834">
+      <c r="G834" s="7"/>
+    </row>
+    <row r="835">
+      <c r="G835" s="7"/>
+    </row>
+    <row r="836">
+      <c r="G836" s="7"/>
+    </row>
+    <row r="837">
+      <c r="G837" s="7"/>
+    </row>
+    <row r="838">
+      <c r="G838" s="7"/>
+    </row>
+    <row r="839">
+      <c r="G839" s="7"/>
+    </row>
+    <row r="840">
+      <c r="G840" s="7"/>
+    </row>
+    <row r="841">
+      <c r="G841" s="7"/>
+    </row>
+    <row r="842">
+      <c r="G842" s="7"/>
+    </row>
+    <row r="843">
+      <c r="G843" s="7"/>
+    </row>
+    <row r="844">
+      <c r="G844" s="7"/>
+    </row>
+    <row r="845">
+      <c r="G845" s="7"/>
+    </row>
+    <row r="846">
+      <c r="G846" s="7"/>
+    </row>
+    <row r="847">
+      <c r="G847" s="7"/>
+    </row>
+    <row r="848">
+      <c r="G848" s="7"/>
+    </row>
+    <row r="849">
+      <c r="G849" s="7"/>
+    </row>
+    <row r="850">
+      <c r="G850" s="7"/>
+    </row>
+    <row r="851">
+      <c r="G851" s="7"/>
+    </row>
+    <row r="852">
+      <c r="G852" s="7"/>
+    </row>
+    <row r="853">
+      <c r="G853" s="7"/>
+    </row>
+    <row r="854">
+      <c r="G854" s="7"/>
+    </row>
+    <row r="855">
+      <c r="G855" s="7"/>
+    </row>
+    <row r="856">
+      <c r="G856" s="7"/>
+    </row>
+    <row r="857">
+      <c r="G857" s="7"/>
+    </row>
+    <row r="858">
+      <c r="G858" s="7"/>
+    </row>
+    <row r="859">
+      <c r="G859" s="7"/>
+    </row>
+    <row r="860">
+      <c r="G860" s="7"/>
+    </row>
+    <row r="861">
+      <c r="G861" s="7"/>
+    </row>
+    <row r="862">
+      <c r="G862" s="7"/>
+    </row>
+    <row r="863">
+      <c r="G863" s="7"/>
+    </row>
+    <row r="864">
+      <c r="G864" s="7"/>
+    </row>
+    <row r="865">
+      <c r="G865" s="7"/>
+    </row>
+    <row r="866">
+      <c r="G866" s="7"/>
+    </row>
+    <row r="867">
+      <c r="G867" s="7"/>
+    </row>
+    <row r="868">
+      <c r="G868" s="7"/>
+    </row>
+    <row r="869">
+      <c r="G869" s="7"/>
+    </row>
+    <row r="870">
+      <c r="G870" s="7"/>
+    </row>
+    <row r="871">
+      <c r="G871" s="7"/>
+    </row>
+    <row r="872">
+      <c r="G872" s="7"/>
+    </row>
+    <row r="873">
+      <c r="G873" s="7"/>
+    </row>
+    <row r="874">
+      <c r="G874" s="7"/>
+    </row>
+    <row r="875">
+      <c r="G875" s="7"/>
+    </row>
+    <row r="876">
+      <c r="G876" s="7"/>
+    </row>
+    <row r="877">
+      <c r="G877" s="7"/>
+    </row>
+    <row r="878">
+      <c r="G878" s="7"/>
+    </row>
+    <row r="879">
+      <c r="G879" s="7"/>
+    </row>
+    <row r="880">
+      <c r="G880" s="7"/>
+    </row>
+    <row r="881">
+      <c r="G881" s="7"/>
+    </row>
+    <row r="882">
+      <c r="G882" s="7"/>
+    </row>
+    <row r="883">
+      <c r="G883" s="7"/>
+    </row>
+    <row r="884">
+      <c r="G884" s="7"/>
+    </row>
+    <row r="885">
+      <c r="G885" s="7"/>
+    </row>
+    <row r="886">
+      <c r="G886" s="7"/>
+    </row>
+    <row r="887">
+      <c r="G887" s="7"/>
+    </row>
+    <row r="888">
+      <c r="G888" s="7"/>
+    </row>
+    <row r="889">
+      <c r="G889" s="7"/>
+    </row>
+    <row r="890">
+      <c r="G890" s="7"/>
+    </row>
+    <row r="891">
+      <c r="G891" s="7"/>
+    </row>
+    <row r="892">
+      <c r="G892" s="7"/>
+    </row>
+    <row r="893">
+      <c r="G893" s="7"/>
+    </row>
+    <row r="894">
+      <c r="G894" s="7"/>
+    </row>
+    <row r="895">
+      <c r="G895" s="7"/>
+    </row>
+    <row r="896">
+      <c r="G896" s="7"/>
+    </row>
+    <row r="897">
+      <c r="G897" s="7"/>
+    </row>
+    <row r="898">
+      <c r="G898" s="7"/>
+    </row>
+    <row r="899">
+      <c r="G899" s="7"/>
+    </row>
+    <row r="900">
+      <c r="G900" s="7"/>
+    </row>
+    <row r="901">
+      <c r="G901" s="7"/>
+    </row>
+    <row r="902">
+      <c r="G902" s="7"/>
+    </row>
+    <row r="903">
+      <c r="G903" s="7"/>
+    </row>
+    <row r="904">
+      <c r="G904" s="7"/>
+    </row>
+    <row r="905">
+      <c r="G905" s="7"/>
+    </row>
+    <row r="906">
+      <c r="G906" s="7"/>
+    </row>
+    <row r="907">
+      <c r="G907" s="7"/>
+    </row>
+    <row r="908">
+      <c r="G908" s="7"/>
+    </row>
+    <row r="909">
+      <c r="G909" s="7"/>
+    </row>
+    <row r="910">
+      <c r="G910" s="7"/>
+    </row>
+    <row r="911">
+      <c r="G911" s="7"/>
+    </row>
+    <row r="912">
+      <c r="G912" s="7"/>
+    </row>
+    <row r="913">
+      <c r="G913" s="7"/>
+    </row>
+    <row r="914">
+      <c r="G914" s="7"/>
+    </row>
+    <row r="915">
+      <c r="G915" s="7"/>
+    </row>
+    <row r="916">
+      <c r="G916" s="7"/>
+    </row>
+    <row r="917">
+      <c r="G917" s="7"/>
+    </row>
+    <row r="918">
+      <c r="G918" s="7"/>
+    </row>
+    <row r="919">
+      <c r="G919" s="7"/>
+    </row>
+    <row r="920">
+      <c r="G920" s="7"/>
+    </row>
+    <row r="921">
+      <c r="G921" s="7"/>
+    </row>
+    <row r="922">
+      <c r="G922" s="7"/>
+    </row>
+    <row r="923">
+      <c r="G923" s="7"/>
+    </row>
+    <row r="924">
+      <c r="G924" s="7"/>
+    </row>
+    <row r="925">
+      <c r="G925" s="7"/>
+    </row>
+    <row r="926">
+      <c r="G926" s="7"/>
+    </row>
+    <row r="927">
+      <c r="G927" s="7"/>
+    </row>
+    <row r="928">
+      <c r="G928" s="7"/>
+    </row>
+    <row r="929">
+      <c r="G929" s="7"/>
+    </row>
+    <row r="930">
+      <c r="G930" s="7"/>
+    </row>
+    <row r="931">
+      <c r="G931" s="7"/>
+    </row>
+    <row r="932">
+      <c r="G932" s="7"/>
+    </row>
+    <row r="933">
+      <c r="G933" s="7"/>
+    </row>
+    <row r="934">
+      <c r="G934" s="7"/>
+    </row>
+    <row r="935">
+      <c r="G935" s="7"/>
+    </row>
+    <row r="936">
+      <c r="G936" s="7"/>
+    </row>
+    <row r="937">
+      <c r="G937" s="7"/>
+    </row>
+    <row r="938">
+      <c r="G938" s="7"/>
+    </row>
+    <row r="939">
+      <c r="G939" s="7"/>
+    </row>
+    <row r="940">
+      <c r="G940" s="7"/>
+    </row>
+    <row r="941">
+      <c r="G941" s="7"/>
+    </row>
+    <row r="942">
+      <c r="G942" s="7"/>
+    </row>
+    <row r="943">
+      <c r="G943" s="7"/>
+    </row>
+    <row r="944">
+      <c r="G944" s="7"/>
+    </row>
+    <row r="945">
+      <c r="G945" s="7"/>
+    </row>
+    <row r="946">
+      <c r="G946" s="7"/>
+    </row>
+    <row r="947">
+      <c r="G947" s="7"/>
+    </row>
+    <row r="948">
+      <c r="G948" s="7"/>
+    </row>
+    <row r="949">
+      <c r="G949" s="7"/>
+    </row>
+    <row r="950">
+      <c r="G950" s="7"/>
+    </row>
+    <row r="951">
+      <c r="G951" s="7"/>
+    </row>
+    <row r="952">
+      <c r="G952" s="7"/>
+    </row>
+    <row r="953">
+      <c r="G953" s="7"/>
+    </row>
+    <row r="954">
+      <c r="G954" s="7"/>
+    </row>
+    <row r="955">
+      <c r="G955" s="7"/>
+    </row>
+    <row r="956">
+      <c r="G956" s="7"/>
+    </row>
+    <row r="957">
+      <c r="G957" s="7"/>
+    </row>
+    <row r="958">
+      <c r="G958" s="7"/>
+    </row>
+    <row r="959">
+      <c r="G959" s="7"/>
+    </row>
+    <row r="960">
+      <c r="G960" s="7"/>
+    </row>
+    <row r="961">
+      <c r="G961" s="7"/>
+    </row>
+    <row r="962">
+      <c r="G962" s="7"/>
+    </row>
+    <row r="963">
+      <c r="G963" s="7"/>
+    </row>
+    <row r="964">
+      <c r="G964" s="7"/>
+    </row>
+    <row r="965">
+      <c r="G965" s="7"/>
+    </row>
+    <row r="966">
+      <c r="G966" s="7"/>
+    </row>
+    <row r="967">
+      <c r="G967" s="7"/>
+    </row>
+    <row r="968">
+      <c r="G968" s="7"/>
+    </row>
+    <row r="969">
+      <c r="G969" s="7"/>
+    </row>
+    <row r="970">
+      <c r="G970" s="7"/>
+    </row>
+    <row r="971">
+      <c r="G971" s="7"/>
+    </row>
+    <row r="972">
+      <c r="G972" s="7"/>
+    </row>
+    <row r="973">
+      <c r="G973" s="7"/>
+    </row>
+    <row r="974">
+      <c r="G974" s="7"/>
+    </row>
+    <row r="975">
+      <c r="G975" s="7"/>
+    </row>
+    <row r="976">
+      <c r="G976" s="7"/>
+    </row>
+    <row r="977">
+      <c r="G977" s="7"/>
+    </row>
+    <row r="978">
+      <c r="G978" s="7"/>
+    </row>
+    <row r="979">
+      <c r="G979" s="7"/>
+    </row>
+    <row r="980">
+      <c r="G980" s="7"/>
+    </row>
+    <row r="981">
+      <c r="G981" s="7"/>
+    </row>
+    <row r="982">
+      <c r="G982" s="7"/>
+    </row>
+    <row r="983">
+      <c r="G983" s="7"/>
+    </row>
+    <row r="984">
+      <c r="G984" s="7"/>
+    </row>
+    <row r="985">
+      <c r="G985" s="7"/>
+    </row>
+    <row r="986">
+      <c r="G986" s="7"/>
+    </row>
+    <row r="987">
+      <c r="G987" s="7"/>
+    </row>
+    <row r="988">
+      <c r="G988" s="7"/>
+    </row>
+    <row r="989">
+      <c r="G989" s="7"/>
+    </row>
+    <row r="990">
+      <c r="G990" s="7"/>
+    </row>
+    <row r="991">
+      <c r="G991" s="7"/>
+    </row>
+    <row r="992">
+      <c r="G992" s="7"/>
+    </row>
+    <row r="993">
+      <c r="G993" s="7"/>
+    </row>
+    <row r="994">
+      <c r="G994" s="7"/>
+    </row>
+    <row r="995">
+      <c r="G995" s="7"/>
+    </row>
+    <row r="996">
+      <c r="G996" s="7"/>
+    </row>
+    <row r="997">
+      <c r="G997" s="7"/>
+    </row>
+    <row r="998">
+      <c r="G998" s="7"/>
+    </row>
+    <row r="999">
+      <c r="G999" s="7"/>
+    </row>
+    <row r="1000">
+      <c r="G1000" s="7"/>
+    </row>
+    <row r="1001">
+      <c r="G1001" s="7"/>
+    </row>
+    <row r="1002">
+      <c r="G1002" s="7"/>
     </row>
   </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" sqref="G1:G1002">
+      <formula1>"Left,Right,Center,HetrisCenter"</formula1>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>